<commit_message>
Ordinati campi di input in interfaccia
</commit_message>
<xml_diff>
--- a/Solution/PptGeneratorGUI/Templates/DataSource_Template.xlsx
+++ b/Solution/PptGeneratorGUI/Templates/DataSource_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16215" tabRatio="851" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16215" tabRatio="851" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Superdettagli" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="238">
   <si>
     <t>da considerare?_</t>
   </si>
@@ -687,12 +687,6 @@
   </si>
   <si>
     <t>PP_12</t>
-  </si>
-  <si>
-    <t>PP_13</t>
-  </si>
-  <si>
-    <t>PP_14</t>
   </si>
   <si>
     <t>Engineering KPI_Sales.pptx</t>
@@ -875,7 +869,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1000,11 +994,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="7"/>
+      </right>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1026,6 +1042,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2814,10 +2832,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -2835,10 +2853,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -3328,10 +3346,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -3349,10 +3367,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -3842,10 +3860,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -3863,10 +3881,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -4356,10 +4374,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -4377,10 +4395,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -4870,10 +4888,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -4891,10 +4909,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -5384,10 +5402,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -5405,10 +5423,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -5898,10 +5916,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -5919,10 +5937,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -6401,7 +6419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -6412,10 +6430,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -6433,10 +6451,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -7408,8 +7426,8 @@
   </sheetPr>
   <dimension ref="A1:Z93"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7426,39 +7444,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="A1" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="K1" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="L1" s="16"/>
+      <c r="K1" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="L1" s="18"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>190</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C3" t="s">
         <v>191</v>
@@ -7475,10 +7493,10 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="K3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -7486,7 +7504,7 @@
         <v>195</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>196</v>
@@ -7501,13 +7519,13 @@
         <v>199</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I4" s="3"/>
-      <c r="K4" t="s">
-        <v>219</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="K4" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="L4" s="16" t="s">
         <v>7</v>
       </c>
     </row>
@@ -7516,7 +7534,7 @@
         <v>195</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>197</v>
@@ -7525,10 +7543,10 @@
       <c r="E5" s="1"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="K5" t="s">
-        <v>219</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="K5" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="L5" s="16" t="s">
         <v>8</v>
       </c>
     </row>
@@ -7537,7 +7555,7 @@
         <v>195</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>200</v>
@@ -7546,10 +7564,10 @@
       <c r="E6" s="1"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="K6" t="s">
-        <v>220</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="K6" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="L6" s="16" t="s">
         <v>156</v>
       </c>
     </row>
@@ -7558,7 +7576,7 @@
         <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>201</v>
@@ -7567,10 +7585,10 @@
       <c r="E7" s="1"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="K7" t="s">
-        <v>220</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="K7" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="L7" s="16" t="s">
         <v>157</v>
       </c>
     </row>
@@ -7579,7 +7597,7 @@
         <v>195</v>
       </c>
       <c r="B8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>202</v>
@@ -7588,11 +7606,11 @@
       <c r="E8" s="1"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="K8" t="s">
-        <v>219</v>
-      </c>
-      <c r="L8" t="s">
-        <v>128</v>
+      <c r="K8" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -7600,7 +7618,7 @@
         <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>198</v>
@@ -7614,10 +7632,10 @@
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="K9" t="s">
-        <v>219</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="K9" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="L9" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7626,7 +7644,7 @@
         <v>195</v>
       </c>
       <c r="B10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>203</v>
@@ -7634,13 +7652,13 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="H10" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="K10" t="s">
-        <v>221</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="K10" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="L10" s="16" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7649,7 +7667,7 @@
         <v>195</v>
       </c>
       <c r="B11" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>204</v>
@@ -7658,11 +7676,11 @@
       <c r="E11" s="1"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="K11" t="s">
-        <v>221</v>
-      </c>
-      <c r="L11" t="s">
-        <v>158</v>
+      <c r="K11" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -7670,7 +7688,7 @@
         <v>195</v>
       </c>
       <c r="B12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>207</v>
@@ -7687,7 +7705,7 @@
         <v>195</v>
       </c>
       <c r="B13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>205</v>
@@ -7704,7 +7722,7 @@
         <v>195</v>
       </c>
       <c r="B14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>208</v>
@@ -7721,7 +7739,7 @@
         <v>195</v>
       </c>
       <c r="B15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>209</v>
@@ -7738,10 +7756,10 @@
         <v>195</v>
       </c>
       <c r="B16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -7755,10 +7773,10 @@
         <v>195</v>
       </c>
       <c r="B17" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>201</v>
@@ -7776,10 +7794,10 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B18" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>196</v>
@@ -7793,13 +7811,13 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B19" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -7810,13 +7828,13 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B20" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -7827,10 +7845,10 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B21" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>201</v>
@@ -7844,10 +7862,10 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B22" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>202</v>
@@ -7859,10 +7877,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B23" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>208</v>
@@ -7874,10 +7892,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B24" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>203</v>
@@ -8345,10 +8363,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -8367,10 +8385,10 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -8906,10 +8924,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -8927,10 +8945,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -9420,10 +9438,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -9441,10 +9459,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -9934,10 +9952,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -9955,10 +9973,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>

</xml_diff>